<commit_message>
Big change up to resource system
</commit_message>
<xml_diff>
--- a/Plotting/RR_ISRU.xlsx
+++ b/Plotting/RR_ISRU.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\RationalResources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Kerbal Space Program\GameData\SkyhawkKerbalism\Plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD7E515-68F8-4705-A367-4B128C78D46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31620" yWindow="0" windowWidth="17700" windowHeight="10485"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="18288" windowHeight="10068" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc (Kg)" sheetId="6" r:id="rId1"/>
     <sheet name="Calc (Moles)" sheetId="7" r:id="rId2"/>
     <sheet name="Database" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="210">
   <si>
     <t>Resource</t>
   </si>
@@ -684,11 +686,26 @@
   <si>
     <t>D+He3</t>
   </si>
+  <si>
+    <t>WasteWater (SK)</t>
+  </si>
+  <si>
+    <t>Water (SK)</t>
+  </si>
+  <si>
+    <t>Food (SK)</t>
+  </si>
+  <si>
+    <t>Waste (SK)</t>
+  </si>
+  <si>
+    <t>Oxygen (SK)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;kg/mol&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.000\ &quot;kg/unit&quot;"/>
@@ -1315,19 +1332,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="18.625" customWidth="1"/>
+    <col min="1" max="6" width="18.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="35" t="s">
         <v>99</v>
       </c>
@@ -1337,22 +1354,22 @@
       <c r="E1" s="35"/>
       <c r="F1" s="35"/>
     </row>
-    <row r="2" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="36" t="s">
         <v>72</v>
       </c>
@@ -1362,12 +1379,12 @@
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>97</v>
       </c>
       <c r="B6" s="18">
-        <v>0</v>
+        <v>4.6296289999999999E-5</v>
       </c>
       <c r="C6" s="18">
         <v>0</v>
@@ -1382,48 +1399,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="27" t="s">
+        <v>208</v>
+      </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="21" t="str">
-        <f>IFERROR(VLOOKUP(B7,Database!$A$2:$E$123,5,FALSE),"-")</f>
-        <v>-</v>
+      <c r="B8" s="21">
+        <f>IFERROR(VLOOKUP(B7,Database!$A$2:$E$128,5,FALSE),"-")</f>
+        <v>0.32500000000000001</v>
       </c>
       <c r="C8" s="21" t="str">
-        <f>IFERROR(VLOOKUP(C7,Database!$A$2:$E$123,5,FALSE),"-")</f>
+        <f>IFERROR(VLOOKUP(C7,Database!$A$2:$E$128,5,FALSE),"-")</f>
         <v>-</v>
       </c>
       <c r="D8" s="21" t="str">
-        <f>IFERROR(VLOOKUP(D7,Database!$A$2:$E$123,5,FALSE),"-")</f>
+        <f>IFERROR(VLOOKUP(D7,Database!$A$2:$E$128,5,FALSE),"-")</f>
         <v>-</v>
       </c>
       <c r="E8" s="21" t="str">
-        <f>IFERROR(VLOOKUP(E7,Database!$A$2:$E$123,5,FALSE),"-")</f>
+        <f>IFERROR(VLOOKUP(E7,Database!$A$2:$E$128,5,FALSE),"-")</f>
         <v>-</v>
       </c>
       <c r="F8" s="21" t="str">
-        <f>IFERROR(VLOOKUP(F7,Database!$A$2:$E$123,5,FALSE),"-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(VLOOKUP(F7,Database!$A$2:$E$128,5,FALSE),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="24" t="str">
+      <c r="B9" s="24">
         <f t="shared" ref="B9:E9" si="0">IFERROR(B6*B8,"-")</f>
-        <v>-</v>
+        <v>1.504629425E-5</v>
       </c>
       <c r="C9" s="24" t="str">
         <f t="shared" si="0"/>
@@ -1442,20 +1461,20 @@
         <v>-</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B10" s="33">
         <f>SUM(B9:F9)</f>
-        <v>0</v>
+        <v>1.504629425E-5</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
     </row>
-    <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="36" t="s">
         <v>73</v>
       </c>
@@ -1465,12 +1484,12 @@
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
     </row>
-    <row r="13" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>97</v>
       </c>
       <c r="B13" s="18">
-        <v>0</v>
+        <v>2.4540774999999999E-5</v>
       </c>
       <c r="C13" s="18">
         <v>0</v>
@@ -1485,56 +1504,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
+      <c r="B14" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>206</v>
+      </c>
       <c r="E14" s="27"/>
       <c r="F14" s="27"/>
     </row>
-    <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="21" t="str">
-        <f>IFERROR(VLOOKUP(B14,Database!$A$2:$E$123,5,FALSE),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="C15" s="21" t="str">
-        <f>IFERROR(VLOOKUP(C14,Database!$A$2:$E$123,5,FALSE),"-")</f>
-        <v>-</v>
-      </c>
-      <c r="D15" s="21" t="str">
-        <f>IFERROR(VLOOKUP(D14,Database!$A$2:$E$123,5,FALSE),"-")</f>
-        <v>-</v>
+      <c r="B15" s="21">
+        <f>IFERROR(VLOOKUP(B14,Database!$A$2:$E$128,5,FALSE),"-")</f>
+        <v>7.6899999999999994E-4</v>
+      </c>
+      <c r="C15" s="21">
+        <f>IFERROR(VLOOKUP(C14,Database!$A$2:$E$128,5,FALSE),"-")</f>
+        <v>0.9</v>
+      </c>
+      <c r="D15" s="21">
+        <f>IFERROR(VLOOKUP(D14,Database!$A$2:$E$128,5,FALSE),"-")</f>
+        <v>0.625</v>
       </c>
       <c r="E15" s="21" t="str">
-        <f>IFERROR(VLOOKUP(E14,Database!$A$2:$E$123,5,FALSE),"-")</f>
+        <f>IFERROR(VLOOKUP(E14,Database!$A$2:$E$128,5,FALSE),"-")</f>
         <v>-</v>
       </c>
       <c r="F15" s="21" t="str">
-        <f>IFERROR(VLOOKUP(F14,Database!$A$2:$E$123,5,FALSE),"-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+        <f>IFERROR(VLOOKUP(F14,Database!$A$2:$E$128,5,FALSE),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="32" t="str">
+      <c r="B16" s="32">
         <f t="shared" ref="B16:E16" si="1">IFERROR(B13*B15,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="C16" s="24" t="str">
+        <v>1.8871855974999997E-8</v>
+      </c>
+      <c r="C16" s="24">
         <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="D16" s="32" t="str">
+        <v>0</v>
+      </c>
+      <c r="D16" s="32">
         <f t="shared" si="1"/>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="E16" s="24" t="str">
         <f t="shared" si="1"/>
@@ -1545,20 +1570,20 @@
         <v>-</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B17" s="33">
         <f>SUM(B16:F16)</f>
-        <v>0</v>
+        <v>1.8871855974999997E-8</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
     </row>
-    <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="37" t="s">
         <v>77</v>
       </c>
@@ -1568,20 +1593,20 @@
       <c r="E19" s="37"/>
       <c r="F19" s="37"/>
     </row>
-    <row r="20" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B20" s="20" t="str">
         <f>IF($B$10&gt;$B$17,"Input excesive",IF($B$10&lt;$B$17,"Output excessive","Equal"))</f>
-        <v>Equal</v>
+        <v>Input excesive</v>
       </c>
       <c r="C20" s="34">
         <f>IF($B$10&gt;$B$17,B10/B17,IF($B$10&lt;$B$17,B17/B10,1))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>797.28746711145891</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
     </row>
   </sheetData>
@@ -1594,18 +1619,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
-            <xm:f>Database!$A$2:$A$123</xm:f>
+            <xm:f>Database!$A$2:$A$128</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:F7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database!$A$2:$A$123</xm:f>
-          </x14:formula1>
-          <xm:sqref>B14:F14</xm:sqref>
+          <xm:sqref>B7:F7 B14:F14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1614,19 +1633,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="18.625" customWidth="1"/>
+    <col min="1" max="6" width="18.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="35" t="s">
         <v>98</v>
       </c>
@@ -1636,22 +1655,22 @@
       <c r="E1" s="35"/>
       <c r="F1" s="35"/>
     </row>
-    <row r="2" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="36" t="s">
         <v>72</v>
       </c>
@@ -1661,7 +1680,7 @@
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>94</v>
       </c>
@@ -1681,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>103</v>
       </c>
@@ -1691,7 +1710,7 @@
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>95</v>
       </c>
@@ -1716,7 +1735,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>100</v>
       </c>
@@ -1741,7 +1760,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>96</v>
       </c>
@@ -1766,7 +1785,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>97</v>
       </c>
@@ -1791,7 +1810,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>101</v>
       </c>
@@ -1800,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="36" t="s">
         <v>73</v>
       </c>
@@ -1810,7 +1829,7 @@
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
     </row>
-    <row r="15" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>94</v>
       </c>
@@ -1830,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>103</v>
       </c>
@@ -1840,7 +1859,7 @@
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
     </row>
-    <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>95</v>
       </c>
@@ -1865,7 +1884,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>100</v>
       </c>
@@ -1890,7 +1909,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>96</v>
       </c>
@@ -1915,7 +1934,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>97</v>
       </c>
@@ -1940,7 +1959,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>101</v>
       </c>
@@ -1949,10 +1968,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="37" t="s">
         <v>77</v>
       </c>
@@ -1962,7 +1981,7 @@
       <c r="E23" s="37"/>
       <c r="F23" s="37"/>
     </row>
-    <row r="24" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>78</v>
       </c>
@@ -1975,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
     </row>
   </sheetData>
@@ -1988,18 +2007,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
-            <xm:f>Database!$A$2:$A$123</xm:f>
+            <xm:f>Database!$A$2:$A$128</xm:f>
           </x14:formula1>
-          <xm:sqref>B16:F16</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database!$A$2:$A$123</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7:F7</xm:sqref>
+          <xm:sqref>B16:F16 B7:F7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2008,26 +2021,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L123"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.25" customWidth="1"/>
-    <col min="2" max="2" width="26.75" customWidth="1"/>
-    <col min="3" max="3" width="13.625" customWidth="1"/>
+    <col min="1" max="1" width="15.19921875" customWidth="1"/>
+    <col min="2" max="2" width="26.69921875" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="18.125" customWidth="1"/>
+    <col min="5" max="5" width="18.09765625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="47.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2047,7 +2060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -2082,7 +2095,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2116,7 +2129,7 @@
         <v>0.69599999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
@@ -2151,7 +2164,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -2186,7 +2199,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -2210,7 +2223,7 @@
       </c>
       <c r="L6" s="22"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>82</v>
       </c>
@@ -2226,7 +2239,7 @@
       <c r="F7" s="6"/>
       <c r="L7" s="22"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I8" t="s">
         <v>88</v>
       </c>
@@ -2237,7 +2250,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>196</v>
       </c>
@@ -2269,7 +2282,7 @@
         <v>1.9599999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -2291,7 +2304,7 @@
         <v>2.5618090452261304E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -2313,7 +2326,7 @@
         <v>9.7400722021660658E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -2335,7 +2348,7 @@
         <v>22.145643693107935</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2357,7 +2370,7 @@
         <v>22.393497757847534</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -2379,7 +2392,7 @@
         <v>5.7190476190476193E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
@@ -2401,7 +2414,7 @@
         <v>22.557662737057917</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>189</v>
       </c>
@@ -2423,7 +2436,7 @@
         <v>22.408000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>128</v>
       </c>
@@ -2438,7 +2451,7 @@
       </c>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>176</v>
       </c>
@@ -2460,7 +2473,7 @@
         <v>1.1078125000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>129</v>
       </c>
@@ -2475,7 +2488,7 @@
       </c>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>170</v>
       </c>
@@ -2497,7 +2510,7 @@
         <v>2.1698268003646309E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>171</v>
       </c>
@@ -2519,7 +2532,7 @@
         <v>11.188888888888888</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>123</v>
       </c>
@@ -2541,7 +2554,7 @@
         <v>3.755E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>130</v>
       </c>
@@ -2563,7 +2576,7 @@
         <v>2.1698268003646309E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>187</v>
       </c>
@@ -2585,7 +2598,7 @@
         <v>5.8390367553865653E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>194</v>
       </c>
@@ -2607,7 +2620,7 @@
         <v>7.2713751113751113E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -2629,7 +2642,7 @@
         <v>7.3551999999999992E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>137</v>
       </c>
@@ -2644,7 +2657,7 @@
       </c>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>155</v>
       </c>
@@ -2659,7 +2672,7 @@
       </c>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>177</v>
       </c>
@@ -2681,7 +2694,7 @@
         <v>5.9375000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>201</v>
       </c>
@@ -2694,7 +2707,7 @@
       </c>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>110</v>
       </c>
@@ -2717,7 +2730,7 @@
         <v>2.3287037037037037E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>145</v>
       </c>
@@ -2739,7 +2752,7 @@
         <v>7.6741666666666668E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -2761,7 +2774,7 @@
         <v>3.1298181818181815E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>183</v>
       </c>
@@ -2783,7 +2796,7 @@
         <v>24.128</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>184</v>
       </c>
@@ -2805,7 +2818,7 @@
         <v>22.407614781634937</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>193</v>
       </c>
@@ -2827,7 +2840,7 @@
         <v>2.3766596785464708E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
@@ -2849,7 +2862,7 @@
         <v>0.11246</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>160</v>
       </c>
@@ -2872,7 +2885,7 @@
         <v>3.1918326693227091E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>68</v>
       </c>
@@ -2895,7 +2908,7 @@
       </c>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>186</v>
       </c>
@@ -2918,7 +2931,7 @@
       </c>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>143</v>
       </c>
@@ -2941,7 +2954,7 @@
       </c>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -2963,7 +2976,7 @@
         <v>2.4255804016521866E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>190</v>
       </c>
@@ -2985,7 +2998,7 @@
         <v>3.5455696202531646E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>24</v>
       </c>
@@ -3007,7 +3020,7 @@
         <v>3.7511186874067751E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>150</v>
       </c>
@@ -3029,7 +3042,7 @@
         <v>1.2401477832512315E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>151</v>
       </c>
@@ -3051,7 +3064,7 @@
         <v>5.1118644067796613E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>182</v>
       </c>
@@ -3073,7 +3086,7 @@
         <v>2.2407614781634933E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>81</v>
       </c>
@@ -3095,7 +3108,7 @@
         <v>2.8510938602681724E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3117,7 +3130,7 @@
         <v>3.7710580108550079E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>79</v>
       </c>
@@ -3139,7 +3152,7 @@
         <v>2.8045574057843997E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>80</v>
       </c>
@@ -3161,7 +3174,7 @@
         <v>3.3955342844708553E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>134</v>
       </c>
@@ -3176,7 +3189,7 @@
       </c>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>124</v>
       </c>
@@ -3191,7 +3204,7 @@
       </c>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>156</v>
       </c>
@@ -3214,7 +3227,7 @@
         <v>2.851093860268172E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>131</v>
       </c>
@@ -3236,7 +3249,7 @@
         <v>2.9034545454545455E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>35</v>
       </c>
@@ -3259,7 +3272,7 @@
         <v>4.2957692307692306E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>83</v>
       </c>
@@ -3282,7 +3295,7 @@
         <v>1.4319230769230768E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>18</v>
       </c>
@@ -3305,7 +3318,7 @@
         <v>22.387726638772666</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>31</v>
       </c>
@@ -3328,7 +3341,7 @@
         <v>3.2656296296296294E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>157</v>
       </c>
@@ -3350,7 +3363,7 @@
         <v>5.2352272727272726E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>41</v>
       </c>
@@ -3372,7 +3385,7 @@
         <v>4.6775999999999998E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>142</v>
       </c>
@@ -3387,7 +3400,7 @@
       </c>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>54</v>
       </c>
@@ -3410,7 +3423,7 @@
         <v>22.393285371702639</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>158</v>
       </c>
@@ -3432,7 +3445,7 @@
         <v>6.3475862068965522E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>154</v>
       </c>
@@ -3446,7 +3459,7 @@
       </c>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>132</v>
       </c>
@@ -3461,7 +3474,7 @@
       </c>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>56</v>
       </c>
@@ -3483,7 +3496,7 @@
         <v>22.695035460992909</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>43</v>
       </c>
@@ -3505,7 +3518,7 @@
         <v>6.1939999999999999E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>126</v>
       </c>
@@ -3520,7 +3533,7 @@
       </c>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>36</v>
       </c>
@@ -3543,7 +3556,7 @@
         <v>2.5010000000000001E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>133</v>
       </c>
@@ -3558,7 +3571,7 @@
       </c>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
@@ -3573,7 +3586,7 @@
       </c>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>146</v>
       </c>
@@ -3588,7 +3601,7 @@
       </c>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>147</v>
       </c>
@@ -3603,7 +3616,7 @@
       </c>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>37</v>
       </c>
@@ -3625,7 +3638,7 @@
         <v>3.0432000000000001E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>174</v>
       </c>
@@ -3647,7 +3660,7 @@
         <v>1.2060970373550882E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>125</v>
       </c>
@@ -3662,7 +3675,7 @@
       </c>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>166</v>
       </c>
@@ -3684,7 +3697,7 @@
         <v>6.0029032258064517E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>38</v>
       </c>
@@ -3699,7 +3712,7 @@
       </c>
       <c r="F79" s="6"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>138</v>
       </c>
@@ -3714,7 +3727,7 @@
       </c>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>135</v>
       </c>
@@ -3736,7 +3749,7 @@
         <v>3.6003999999999994E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>159</v>
       </c>
@@ -3758,7 +3771,7 @@
         <v>7.5979772439949439E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>162</v>
       </c>
@@ -3781,7 +3794,7 @@
         <v>6.4036791314837152E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>202</v>
       </c>
@@ -3796,7 +3809,7 @@
       </c>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>203</v>
       </c>
@@ -3811,7 +3824,7 @@
       </c>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>121</v>
       </c>
@@ -3833,286 +3846,307 @@
         <v>1.8020000000000001E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1">
+        <v>1</v>
+      </c>
+      <c r="D87" s="5"/>
+      <c r="E87" s="4">
+        <f>0.000625*1000</f>
+        <v>0.625</v>
+      </c>
+      <c r="F87" s="6"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1</v>
+      </c>
+      <c r="D88" s="5">
+        <v>18.02</v>
+      </c>
+      <c r="E88" s="4">
+        <f>0.000625*1000</f>
+        <v>0.625</v>
+      </c>
+      <c r="F88" s="6">
+        <f>C88*D88/(E88 * 1000)</f>
+        <v>2.8832E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="4">
+        <f xml:space="preserve"> 0.000325*1000</f>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1">
+        <v>1</v>
+      </c>
+      <c r="D90" s="5"/>
+      <c r="E90" s="4">
+        <f>0.000325*1000</f>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="F90" s="6"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="1">
+        <v>1</v>
+      </c>
+      <c r="D91" s="5">
+        <v>32</v>
+      </c>
+      <c r="E91" s="4">
+        <f>0.0000013889*1000</f>
+        <v>1.3889E-3</v>
+      </c>
+      <c r="F91" s="6">
+        <f>C91*D91/(E91 * 1000)</f>
+        <v>23.039815681474547</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="30" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D89" s="31"/>
-      <c r="E89" s="4">
-        <f t="shared" ref="E89:E123" si="11">F89*1000</f>
+      <c r="D94" s="31"/>
+      <c r="E94" s="4">
+        <f t="shared" ref="E94:E128" si="11">F94*1000</f>
         <v>5</v>
       </c>
-      <c r="F89" s="6">
+      <c r="F94" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="30" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="E90" s="4">
+      <c r="E95" s="4">
         <f t="shared" si="11"/>
         <v>19.3</v>
       </c>
-      <c r="F90" s="6">
+      <c r="F95" s="6">
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="30" t="s">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E91" s="4">
+      <c r="E96" s="4">
         <f t="shared" si="11"/>
         <v>54.4</v>
       </c>
-      <c r="F91" s="6">
+      <c r="F96" s="6">
         <v>5.4399999999999997E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="30" t="s">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="E92" s="4">
+      <c r="E97" s="4">
         <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="F92" s="6">
+      <c r="F97" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="30" t="s">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="E93" s="4">
+      <c r="E98" s="4">
         <f t="shared" si="11"/>
         <v>7</v>
       </c>
-      <c r="F93" s="6">
+      <c r="F98" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="30" t="s">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="E94" s="4">
+      <c r="E99" s="4">
         <f t="shared" si="11"/>
         <v>0.53399999999999992</v>
       </c>
-      <c r="F94" s="6">
+      <c r="F99" s="6">
         <v>5.3399999999999997E-4</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="30" t="s">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="E95" s="4">
+      <c r="E100" s="4">
         <f t="shared" si="11"/>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="F95" s="6">
+      <c r="F100" s="6">
         <v>6.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="30" t="s">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="E96" s="4">
+      <c r="E101" s="4">
         <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
-      <c r="F96" s="6">
+      <c r="F101" s="6">
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="30" t="s">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="E97" s="4">
+      <c r="E102" s="4">
         <f t="shared" si="11"/>
         <v>5.0108799999999993</v>
       </c>
-      <c r="F97" s="6">
+      <c r="F102" s="6">
         <v>5.0108799999999997E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="30" t="s">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="E98" s="4">
+      <c r="E103" s="4">
         <f t="shared" si="11"/>
         <v>4.3499999999999996</v>
       </c>
-      <c r="F98" s="6">
+      <c r="F103" s="6">
         <v>4.3499999999999997E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="30" t="s">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="E99" s="4">
+      <c r="E104" s="4">
         <f t="shared" si="11"/>
         <v>0.216</v>
       </c>
-      <c r="F99" s="6">
+      <c r="F104" s="6">
         <v>2.1599999999999999E-4</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="30" t="s">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E100" s="4">
+      <c r="E105" s="4">
         <f t="shared" si="11"/>
         <v>23.125</v>
       </c>
-      <c r="F100" s="6">
+      <c r="F105" s="6">
         <v>2.3125E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="30" t="s">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E101" s="4">
+      <c r="E106" s="4">
         <f t="shared" si="11"/>
         <v>5.25</v>
       </c>
-      <c r="F101" s="6">
+      <c r="F106" s="6">
         <v>5.2500000000000003E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="30" t="s">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E102" s="4">
+      <c r="E107" s="4">
         <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="F102" s="6">
+      <c r="F107" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="30" t="s">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="E103" s="4">
+      <c r="E108" s="4">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="F103" s="6">
+      <c r="F108" s="6">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="30" t="s">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E104" s="4">
+      <c r="E109" s="4">
         <f t="shared" si="11"/>
         <v>12.5</v>
       </c>
-      <c r="F104" s="6">
+      <c r="F109" s="6">
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="E105" s="4">
+      <c r="E110" s="4">
         <f t="shared" si="11"/>
         <v>2.4</v>
       </c>
-      <c r="F105" s="6">
+      <c r="F110" s="6">
         <v>2.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="30" t="s">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="E106" s="4">
-        <f t="shared" si="11"/>
-        <v>13.5</v>
-      </c>
-      <c r="F106" s="6">
-        <v>1.35E-2</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E107" s="4">
-        <f t="shared" si="11"/>
-        <v>8.6</v>
-      </c>
-      <c r="F107" s="6">
-        <v>8.6E-3</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="30" t="s">
-        <v>172</v>
-      </c>
-      <c r="E108" s="4">
-        <f t="shared" si="11"/>
-        <v>19.099999999999998</v>
-      </c>
-      <c r="F108" s="6">
-        <v>1.9099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="E109" s="4">
-        <f t="shared" si="11"/>
-        <v>10.97</v>
-      </c>
-      <c r="F109" s="6">
-        <v>1.0970000000000001E-2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="4">
-        <f t="shared" si="11"/>
-        <v>5.7050000000000001</v>
-      </c>
-      <c r="F110" s="6">
-        <v>5.705E-3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
-      <c r="D111" s="3"/>
       <c r="E111" s="4">
         <f t="shared" si="11"/>
         <v>13.5</v>
@@ -4121,159 +4155,225 @@
         <v>1.35E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="3"/>
+        <v>63</v>
+      </c>
       <c r="E112" s="4">
         <f t="shared" si="11"/>
-        <v>0.35399999999999998</v>
+        <v>8.6</v>
       </c>
       <c r="F112" s="6">
-        <v>3.5399999999999999E-4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8.6E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1"/>
-      <c r="D113" s="3"/>
+        <v>172</v>
+      </c>
       <c r="E113" s="4">
         <f t="shared" si="11"/>
-        <v>2.12805</v>
+        <v>19.099999999999998</v>
       </c>
       <c r="F113" s="6">
-        <v>2.1280499999999998E-3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.9099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="3"/>
+        <v>173</v>
+      </c>
       <c r="E114" s="4">
         <f t="shared" si="11"/>
-        <v>1.08</v>
+        <v>10.97</v>
       </c>
       <c r="F114" s="6">
-        <v>1.08E-3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.0970000000000001E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="30" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="3"/>
       <c r="E115" s="4">
         <f t="shared" si="11"/>
-        <v>4.1000000000000005</v>
+        <v>5.7050000000000001</v>
       </c>
       <c r="F115" s="6">
-        <v>4.1000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.705E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="30" t="s">
-        <v>52</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="3"/>
       <c r="E116" s="4">
         <f t="shared" si="11"/>
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="F116" s="6">
-        <v>1.2500000000000001E-2</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.35E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="30" t="s">
-        <v>71</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="3"/>
       <c r="E117" s="4">
         <f t="shared" si="11"/>
-        <v>4.5999999999999996</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="F117" s="6">
-        <v>4.5999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.5399999999999999E-4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="30" t="s">
-        <v>119</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="3"/>
       <c r="E118" s="4">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>2.12805</v>
       </c>
       <c r="F118" s="6">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.1280499999999998E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="30" t="s">
-        <v>120</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="3"/>
       <c r="E119" s="4">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>1.08</v>
       </c>
       <c r="F119" s="6">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.08E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="30" t="s">
-        <v>114</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="3"/>
       <c r="E120" s="4">
         <f t="shared" si="11"/>
-        <v>7.5</v>
+        <v>4.1000000000000005</v>
       </c>
       <c r="F120" s="6">
-        <v>7.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4.1000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="30" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="E121" s="4">
         <f t="shared" si="11"/>
-        <v>4.3499999999999996</v>
+        <v>12.5</v>
       </c>
       <c r="F121" s="6">
-        <v>4.3499999999999997E-3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="30" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="E122" s="4">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F122" s="6">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="30" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="E123" s="4">
         <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F123" s="6">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E124" s="4">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F124" s="6">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E125" s="4">
+        <f t="shared" si="11"/>
+        <v>7.5</v>
+      </c>
+      <c r="F125" s="6">
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E126" s="4">
+        <f t="shared" si="11"/>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F126" s="6">
+        <v>4.3499999999999997E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E127" s="4">
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="F123" s="6">
+      <c r="F127" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E128" s="4">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="F128" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>

</xml_diff>